<commit_message>
updated stability voltage profiles
</commit_message>
<xml_diff>
--- a/measurement_files/Fig5_6/Measurements details.xlsx
+++ b/measurement_files/Fig5_6/Measurements details.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abedj/Desktop/voltage_profile_stability_testing/measurement_files/Fig5_6/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abedj/Library/CloudStorage/OneDrive-UniversityofToronto/UofT/Research/Publications/Opentrons_paper/AMPERE_repo/measurement_files/Fig5_6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF3E9FF-E6E4-3541-8D2E-1A0C74808D58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB08D6E0-3CA8-6743-9A7F-DE90691197EC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9560" yWindow="2120" windowWidth="24400" windowHeight="17900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-38400" yWindow="-1460" windowWidth="19420" windowHeight="20980" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -84,9 +84,6 @@
     <t>sample number</t>
   </si>
   <si>
-    <t>repeated</t>
-  </si>
-  <si>
     <t>Fig. 5b</t>
   </si>
   <si>
@@ -112,6 +109,9 @@
   </si>
   <si>
     <t>Ethanol concentration [v/v%]</t>
+  </si>
+  <si>
+    <t>repeat</t>
   </si>
 </sst>
 </file>
@@ -160,13 +160,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -448,24 +451,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H100"/>
+  <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="H40" sqref="H40"/>
+    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
+      <selection activeCell="G59" sqref="G59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="8.83203125" style="1"/>
     <col min="3" max="3" width="10.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.5" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="33.5" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.1640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.83203125" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>7</v>
       </c>
@@ -476,13 +480,13 @@
         <v>4</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>5</v>
@@ -491,9 +495,9 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -502,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E2" s="1">
         <v>40</v>
@@ -511,12 +515,12 @@
         <v>20</v>
       </c>
       <c r="H2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -525,7 +529,7 @@
         <v>0</v>
       </c>
       <c r="D3" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E3" s="1">
         <v>40</v>
@@ -534,12 +538,12 @@
         <v>20</v>
       </c>
       <c r="H3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1">
         <v>3</v>
@@ -548,7 +552,7 @@
         <v>0</v>
       </c>
       <c r="D4" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E4" s="1">
         <v>40</v>
@@ -557,10 +561,10 @@
         <v>20</v>
       </c>
       <c r="H4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -580,10 +584,10 @@
         <v>20</v>
       </c>
       <c r="H5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -603,10 +607,10 @@
         <v>20</v>
       </c>
       <c r="H6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -626,12 +630,12 @@
         <v>20</v>
       </c>
       <c r="H7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="1">
         <v>7</v>
@@ -640,7 +644,7 @@
         <v>2</v>
       </c>
       <c r="D8" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E8" s="1">
         <v>40</v>
@@ -649,12 +653,12 @@
         <v>20</v>
       </c>
       <c r="H8" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>8</v>
@@ -663,7 +667,7 @@
         <v>2</v>
       </c>
       <c r="D9" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E9" s="1">
         <v>40</v>
@@ -672,12 +676,12 @@
         <v>20</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1">
         <v>9</v>
@@ -686,7 +690,7 @@
         <v>2</v>
       </c>
       <c r="D10" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E10" s="1">
         <v>40</v>
@@ -695,10 +699,10 @@
         <v>20</v>
       </c>
       <c r="H10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>8</v>
       </c>
@@ -718,10 +722,10 @@
         <v>20</v>
       </c>
       <c r="H11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -741,10 +745,10 @@
         <v>20</v>
       </c>
       <c r="H12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -764,18 +768,18 @@
         <v>20</v>
       </c>
       <c r="H13" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B14" s="1">
         <v>1</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14" s="1">
         <v>20</v>
@@ -784,21 +788,22 @@
         <v>40</v>
       </c>
       <c r="F14" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="I14" s="3"/>
+    </row>
+    <row r="15" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B15" s="1">
         <v>2</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D15" s="1">
         <v>20</v>
@@ -807,21 +812,22 @@
         <v>40</v>
       </c>
       <c r="F15" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H15" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" ht="16" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="I15" s="3"/>
+    </row>
+    <row r="16" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B16" s="1">
         <v>3</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D16" s="1">
         <v>20</v>
@@ -830,13 +836,14 @@
         <v>40</v>
       </c>
       <c r="F16" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H16" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.2">
+        <v>19</v>
+      </c>
+      <c r="I16" s="3"/>
+    </row>
+    <row r="17" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>9</v>
       </c>
@@ -844,22 +851,23 @@
         <v>4</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D17" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E17" s="1">
         <v>40</v>
       </c>
       <c r="F17" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="I17" s="3"/>
+    </row>
+    <row r="18" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>9</v>
       </c>
@@ -867,22 +875,23 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D18" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E18" s="1">
         <v>40</v>
       </c>
       <c r="F18" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H18" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="I18" s="3"/>
+    </row>
+    <row r="19" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>9</v>
       </c>
@@ -890,91 +899,95 @@
         <v>6</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D19" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E19" s="1">
         <v>40</v>
       </c>
       <c r="F19" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H19" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="I19" s="3"/>
+    </row>
+    <row r="20" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B20" s="1">
         <v>4</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D20" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E20" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F20" s="1">
         <v>20</v>
       </c>
       <c r="H20" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="I20" s="3"/>
+    </row>
+    <row r="21" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B21" s="1">
         <v>5</v>
       </c>
       <c r="C21" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D21" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E21" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F21" s="1">
         <v>20</v>
       </c>
       <c r="H21" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="I21" s="3"/>
+    </row>
+    <row r="22" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B22" s="1">
         <v>6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D22" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E22" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F22" s="1">
         <v>20</v>
       </c>
       <c r="H22" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="I22" s="3"/>
+    </row>
+    <row r="23" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>9</v>
       </c>
@@ -982,22 +995,23 @@
         <v>10</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D23" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E23" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F23" s="1">
         <v>20</v>
       </c>
       <c r="H23" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="I23" s="3"/>
+    </row>
+    <row r="24" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>9</v>
       </c>
@@ -1005,22 +1019,23 @@
         <v>11</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D24" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E24" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F24" s="1">
         <v>20</v>
       </c>
       <c r="H24" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="I24" s="3"/>
+    </row>
+    <row r="25" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>9</v>
       </c>
@@ -1028,22 +1043,23 @@
         <v>12</v>
       </c>
       <c r="C25" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D25" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="E25" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F25" s="1">
         <v>20</v>
       </c>
       <c r="H25" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.2">
+        <v>21</v>
+      </c>
+      <c r="I25" s="3"/>
+    </row>
+    <row r="26" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>9</v>
       </c>
@@ -1051,22 +1067,23 @@
         <v>13</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D26" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E26" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F26" s="1">
         <v>20</v>
       </c>
       <c r="H26" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="I26" s="3"/>
+    </row>
+    <row r="27" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>9</v>
       </c>
@@ -1074,22 +1091,23 @@
         <v>14</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D27" s="1">
-        <v>30</v>
+        <v>20</v>
       </c>
       <c r="E27" s="1">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F27" s="1">
         <v>20</v>
       </c>
       <c r="H27" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="I27" s="3"/>
+    </row>
+    <row r="28" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1097,45 +1115,47 @@
         <v>15</v>
       </c>
       <c r="C28" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D28" s="1">
+        <v>20</v>
+      </c>
+      <c r="E28" s="1">
+        <v>20</v>
+      </c>
+      <c r="F28" s="1">
+        <v>20</v>
+      </c>
+      <c r="H28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="3"/>
+    </row>
+    <row r="29" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="1">
+        <v>1</v>
+      </c>
+      <c r="C29" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D28" s="1">
-        <v>30</v>
-      </c>
-      <c r="E28" s="1">
-        <v>40</v>
-      </c>
-      <c r="F28" s="1">
-        <v>20</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="D29" s="1">
+        <v>10</v>
+      </c>
+      <c r="E29" s="1">
+        <v>40</v>
+      </c>
+      <c r="F29" s="1">
+        <v>20</v>
+      </c>
+      <c r="H29" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A29" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="1">
-        <v>1</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D29" s="1">
-        <v>30</v>
-      </c>
-      <c r="E29" s="1">
-        <v>40</v>
-      </c>
-      <c r="F29" s="1">
-        <v>20</v>
-      </c>
-      <c r="H29" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I29" s="3"/>
+    </row>
+    <row r="30" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -1143,10 +1163,10 @@
         <v>2</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D30" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E30" s="1">
         <v>40</v>
@@ -1155,10 +1175,11 @@
         <v>20</v>
       </c>
       <c r="H30" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I30" s="3"/>
+    </row>
+    <row r="31" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -1166,10 +1187,10 @@
         <v>3</v>
       </c>
       <c r="C31" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D31" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E31" s="1">
         <v>40</v>
@@ -1178,21 +1199,22 @@
         <v>20</v>
       </c>
       <c r="H31" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I31" s="3"/>
+    </row>
+    <row r="32" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B32" s="1">
         <v>7</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D32" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E32" s="1">
         <v>40</v>
@@ -1201,21 +1223,22 @@
         <v>20</v>
       </c>
       <c r="H32" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I32" s="3"/>
+    </row>
+    <row r="33" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B33" s="1">
         <v>8</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D33" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E33" s="1">
         <v>40</v>
@@ -1224,21 +1247,22 @@
         <v>20</v>
       </c>
       <c r="H33" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I33" s="3"/>
+    </row>
+    <row r="34" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B34" s="1">
         <v>9</v>
       </c>
       <c r="C34" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D34" s="1">
-        <v>20</v>
+        <v>10</v>
       </c>
       <c r="E34" s="1">
         <v>40</v>
@@ -1247,10 +1271,11 @@
         <v>20</v>
       </c>
       <c r="H34" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I34" s="3"/>
+    </row>
+    <row r="35" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -1258,10 +1283,10 @@
         <v>7</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D35" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E35" s="1">
         <v>40</v>
@@ -1270,10 +1295,11 @@
         <v>20</v>
       </c>
       <c r="H35" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I35" s="3"/>
+    </row>
+    <row r="36" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -1281,10 +1307,10 @@
         <v>8</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D36" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E36" s="1">
         <v>40</v>
@@ -1293,10 +1319,11 @@
         <v>20</v>
       </c>
       <c r="H36" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I36" s="3"/>
+    </row>
+    <row r="37" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -1304,10 +1331,10 @@
         <v>9</v>
       </c>
       <c r="C37" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D37" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E37" s="1">
         <v>40</v>
@@ -1316,33 +1343,35 @@
         <v>20</v>
       </c>
       <c r="H37" t="s">
+        <v>16</v>
+      </c>
+      <c r="I37" s="3"/>
+    </row>
+    <row r="38" spans="1:9" ht="16" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="1">
+        <v>10</v>
+      </c>
+      <c r="C38" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1">
+        <v>10</v>
+      </c>
+      <c r="E38" s="1">
+        <v>40</v>
+      </c>
+      <c r="F38" s="1">
+        <v>20</v>
+      </c>
+      <c r="H38" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A38" t="s">
-        <v>10</v>
-      </c>
-      <c r="B38" s="1">
-        <v>10</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D38" s="1">
-        <v>30</v>
-      </c>
-      <c r="E38" s="1">
-        <v>40</v>
-      </c>
-      <c r="F38" s="1">
-        <v>20</v>
-      </c>
-      <c r="G38" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="I38" s="3"/>
+    </row>
+    <row r="39" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -1350,10 +1379,10 @@
         <v>11</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D39" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E39" s="1">
         <v>40</v>
@@ -1361,11 +1390,12 @@
       <c r="F39" s="1">
         <v>20</v>
       </c>
-      <c r="G39" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H39" t="s">
+        <v>15</v>
+      </c>
+      <c r="I39" s="3"/>
+    </row>
+    <row r="40" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -1373,10 +1403,10 @@
         <v>12</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D40" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="E40" s="1">
         <v>40</v>
@@ -1384,356 +1414,372 @@
       <c r="F40" s="1">
         <v>20</v>
       </c>
-      <c r="G40" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="H40" t="s">
+        <v>15</v>
+      </c>
+      <c r="I40" s="3"/>
+    </row>
+    <row r="41" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B41" s="1">
-        <v>1</v>
+        <v>13</v>
       </c>
       <c r="C41" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D41" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E41" s="1">
         <v>40</v>
       </c>
       <c r="F41" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H41" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I41" s="3"/>
+    </row>
+    <row r="42" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B42" s="1">
-        <v>2</v>
+        <v>14</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D42" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E42" s="1">
         <v>40</v>
       </c>
       <c r="F42" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H42" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I42" s="3"/>
+    </row>
+    <row r="43" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B43" s="1">
-        <v>3</v>
+        <v>15</v>
       </c>
       <c r="C43" s="1" t="s">
         <v>0</v>
       </c>
       <c r="D43" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E43" s="1">
         <v>40</v>
       </c>
       <c r="F43" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H43" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I43" s="3"/>
+    </row>
+    <row r="44" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>11</v>
       </c>
       <c r="B44" s="1">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C44" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D44" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E44" s="1">
         <v>40</v>
       </c>
       <c r="F44" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H44" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I44" s="3"/>
+    </row>
+    <row r="45" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>11</v>
       </c>
       <c r="B45" s="1">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D45" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E45" s="1">
         <v>40</v>
       </c>
       <c r="F45" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H45" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I45" s="3"/>
+    </row>
+    <row r="46" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>11</v>
       </c>
       <c r="B46" s="1">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D46" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E46" s="1">
         <v>40</v>
       </c>
       <c r="F46" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H46" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I46" s="3"/>
+    </row>
+    <row r="47" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>11</v>
       </c>
       <c r="B47" s="1">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D47" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E47" s="1">
         <v>40</v>
       </c>
       <c r="F47" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H47" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I47" s="3"/>
+    </row>
+    <row r="48" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>11</v>
       </c>
       <c r="B48" s="1">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C48" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D48" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E48" s="1">
         <v>40</v>
       </c>
       <c r="F48" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H48" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I48" s="3"/>
+    </row>
+    <row r="49" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>11</v>
       </c>
       <c r="B49" s="1">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="C49" s="1" t="s">
         <v>2</v>
       </c>
       <c r="D49" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E49" s="1">
         <v>40</v>
       </c>
       <c r="F49" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H49" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+        <v>16</v>
+      </c>
+      <c r="I49" s="3"/>
+    </row>
+    <row r="50" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>11</v>
       </c>
       <c r="B50" s="1">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C50" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D50" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E50" s="1">
         <v>40</v>
       </c>
       <c r="F50" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H50" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I50" s="3"/>
+    </row>
+    <row r="51" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>11</v>
       </c>
       <c r="B51" s="1">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="C51" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D51" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E51" s="1">
         <v>40</v>
       </c>
       <c r="F51" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H51" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I51" s="3"/>
+    </row>
+    <row r="52" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>11</v>
       </c>
       <c r="B52" s="1">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C52" s="1" t="s">
         <v>3</v>
       </c>
       <c r="D52" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E52" s="1">
         <v>40</v>
       </c>
       <c r="F52" s="1">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H52" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.2">
+        <v>15</v>
+      </c>
+      <c r="I52" s="3"/>
+    </row>
+    <row r="53" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>11</v>
       </c>
       <c r="B53" s="1">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D53" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E53" s="1">
         <v>40</v>
       </c>
       <c r="F53" s="1">
-        <v>30</v>
-      </c>
-      <c r="H53" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G53" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I53" s="3"/>
+    </row>
+    <row r="54" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>11</v>
       </c>
       <c r="B54" s="1">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D54" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E54" s="1">
         <v>40</v>
       </c>
       <c r="F54" s="1">
-        <v>30</v>
-      </c>
-      <c r="H54" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G54" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I54" s="3"/>
+    </row>
+    <row r="55" spans="1:9" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>11</v>
       </c>
       <c r="B55" s="1">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D55" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="E55" s="1">
         <v>40</v>
       </c>
       <c r="F55" s="1">
-        <v>30</v>
-      </c>
-      <c r="H55" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.2">
+        <v>20</v>
+      </c>
+      <c r="G55" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="I55" s="3"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>12</v>
       </c>
@@ -1741,7 +1787,7 @@
         <v>1</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D56" s="1">
         <v>20</v>
@@ -1750,13 +1796,13 @@
         <v>40</v>
       </c>
       <c r="F56" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H56" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>12</v>
       </c>
@@ -1764,7 +1810,7 @@
         <v>2</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D57" s="1">
         <v>20</v>
@@ -1773,13 +1819,13 @@
         <v>40</v>
       </c>
       <c r="F57" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H57" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>12</v>
       </c>
@@ -1787,7 +1833,7 @@
         <v>3</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58" s="1">
         <v>20</v>
@@ -1796,13 +1842,13 @@
         <v>40</v>
       </c>
       <c r="F58" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H58" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>12</v>
       </c>
@@ -1810,7 +1856,7 @@
         <v>4</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D59" s="1">
         <v>20</v>
@@ -1819,13 +1865,13 @@
         <v>40</v>
       </c>
       <c r="F59" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H59" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>12</v>
       </c>
@@ -1833,7 +1879,7 @@
         <v>5</v>
       </c>
       <c r="C60" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D60" s="1">
         <v>20</v>
@@ -1842,13 +1888,13 @@
         <v>40</v>
       </c>
       <c r="F60" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H60" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>12</v>
       </c>
@@ -1856,7 +1902,7 @@
         <v>6</v>
       </c>
       <c r="C61" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D61" s="1">
         <v>20</v>
@@ -1865,13 +1911,13 @@
         <v>40</v>
       </c>
       <c r="F61" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H61" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>12</v>
       </c>
@@ -1879,7 +1925,7 @@
         <v>7</v>
       </c>
       <c r="C62" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D62" s="1">
         <v>20</v>
@@ -1888,13 +1934,13 @@
         <v>40</v>
       </c>
       <c r="F62" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H62" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>12</v>
       </c>
@@ -1902,7 +1948,7 @@
         <v>8</v>
       </c>
       <c r="C63" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D63" s="1">
         <v>20</v>
@@ -1911,13 +1957,13 @@
         <v>40</v>
       </c>
       <c r="F63" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H63" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>12</v>
       </c>
@@ -1925,7 +1971,7 @@
         <v>9</v>
       </c>
       <c r="C64" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D64" s="1">
         <v>20</v>
@@ -1934,7 +1980,7 @@
         <v>40</v>
       </c>
       <c r="F64" s="1">
-        <v>30</v>
+        <v>10</v>
       </c>
       <c r="H64" t="s">
         <v>19</v>
@@ -1948,7 +1994,7 @@
         <v>10</v>
       </c>
       <c r="C65" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D65" s="1">
         <v>20</v>
@@ -1957,10 +2003,10 @@
         <v>40</v>
       </c>
       <c r="F65" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H65" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.2">
@@ -1971,7 +2017,7 @@
         <v>11</v>
       </c>
       <c r="C66" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D66" s="1">
         <v>20</v>
@@ -1980,10 +2026,10 @@
         <v>40</v>
       </c>
       <c r="F66" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H66" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.2">
@@ -1994,7 +2040,7 @@
         <v>12</v>
       </c>
       <c r="C67" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D67" s="1">
         <v>20</v>
@@ -2003,10 +2049,10 @@
         <v>40</v>
       </c>
       <c r="F67" s="1">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H67" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
@@ -2017,7 +2063,7 @@
         <v>13</v>
       </c>
       <c r="C68" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D68" s="1">
         <v>20</v>
@@ -2026,7 +2072,7 @@
         <v>40</v>
       </c>
       <c r="F68" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H68" t="s">
         <v>19</v>
@@ -2040,7 +2086,7 @@
         <v>14</v>
       </c>
       <c r="C69" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D69" s="1">
         <v>20</v>
@@ -2049,7 +2095,7 @@
         <v>40</v>
       </c>
       <c r="F69" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H69" t="s">
         <v>19</v>
@@ -2063,7 +2109,7 @@
         <v>15</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D70" s="1">
         <v>20</v>
@@ -2072,7 +2118,7 @@
         <v>40</v>
       </c>
       <c r="F70" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H70" t="s">
         <v>19</v>
@@ -2086,7 +2132,7 @@
         <v>1</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D71" s="1">
         <v>20</v>
@@ -2095,10 +2141,10 @@
         <v>40</v>
       </c>
       <c r="F71" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H71" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.2">
@@ -2109,7 +2155,7 @@
         <v>2</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D72" s="1">
         <v>20</v>
@@ -2118,10 +2164,10 @@
         <v>40</v>
       </c>
       <c r="F72" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H72" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.2">
@@ -2132,7 +2178,7 @@
         <v>3</v>
       </c>
       <c r="C73" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D73" s="1">
         <v>20</v>
@@ -2141,10 +2187,10 @@
         <v>40</v>
       </c>
       <c r="F73" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H73" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.2">
@@ -2155,7 +2201,7 @@
         <v>4</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D74" s="1">
         <v>20</v>
@@ -2164,7 +2210,7 @@
         <v>40</v>
       </c>
       <c r="F74" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H74" t="s">
         <v>19</v>
@@ -2178,7 +2224,7 @@
         <v>5</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D75" s="1">
         <v>20</v>
@@ -2187,7 +2233,7 @@
         <v>40</v>
       </c>
       <c r="F75" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H75" t="s">
         <v>19</v>
@@ -2201,7 +2247,7 @@
         <v>6</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D76" s="1">
         <v>20</v>
@@ -2210,7 +2256,7 @@
         <v>40</v>
       </c>
       <c r="F76" s="1">
-        <v>40</v>
+        <v>30</v>
       </c>
       <c r="H76" t="s">
         <v>19</v>
@@ -2224,19 +2270,19 @@
         <v>7</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D77" s="1">
         <v>20</v>
       </c>
       <c r="E77" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F77" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H77" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.2">
@@ -2247,19 +2293,19 @@
         <v>8</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D78" s="1">
         <v>20</v>
       </c>
       <c r="E78" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F78" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H78" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.2">
@@ -2270,19 +2316,19 @@
         <v>9</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="D79" s="1">
         <v>20</v>
       </c>
       <c r="E79" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F79" s="1">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="H79" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.2">
@@ -2293,19 +2339,19 @@
         <v>10</v>
       </c>
       <c r="C80" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D80" s="1">
         <v>20</v>
       </c>
       <c r="E80" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F80" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H80" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.2">
@@ -2316,19 +2362,19 @@
         <v>11</v>
       </c>
       <c r="C81" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D81" s="1">
         <v>20</v>
       </c>
       <c r="E81" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F81" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H81" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.2">
@@ -2339,19 +2385,19 @@
         <v>12</v>
       </c>
       <c r="C82" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D82" s="1">
         <v>20</v>
       </c>
       <c r="E82" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F82" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H82" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.2">
@@ -2362,19 +2408,19 @@
         <v>13</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D83" s="1">
         <v>20</v>
       </c>
       <c r="E83" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F83" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H83" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.2">
@@ -2385,19 +2431,19 @@
         <v>14</v>
       </c>
       <c r="C84" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D84" s="1">
         <v>20</v>
       </c>
       <c r="E84" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F84" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H84" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.2">
@@ -2408,19 +2454,19 @@
         <v>15</v>
       </c>
       <c r="C85" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D85" s="1">
         <v>20</v>
       </c>
       <c r="E85" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F85" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="H85" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.2">
@@ -2443,7 +2489,7 @@
         <v>20</v>
       </c>
       <c r="H86" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.2">
@@ -2466,7 +2512,7 @@
         <v>20</v>
       </c>
       <c r="H87" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.2">
@@ -2489,7 +2535,7 @@
         <v>20</v>
       </c>
       <c r="H88" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.2">
@@ -2512,7 +2558,7 @@
         <v>20</v>
       </c>
       <c r="H89" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.2">
@@ -2535,7 +2581,7 @@
         <v>20</v>
       </c>
       <c r="H90" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.2">
@@ -2558,7 +2604,7 @@
         <v>20</v>
       </c>
       <c r="H91" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.2">
@@ -2581,7 +2627,7 @@
         <v>20</v>
       </c>
       <c r="H92" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.2">
@@ -2604,7 +2650,7 @@
         <v>20</v>
       </c>
       <c r="H93" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.2">
@@ -2627,7 +2673,7 @@
         <v>20</v>
       </c>
       <c r="H94" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.2">
@@ -2650,7 +2696,7 @@
         <v>20</v>
       </c>
       <c r="H95" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.2">
@@ -2673,7 +2719,7 @@
         <v>20</v>
       </c>
       <c r="H96" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.2">
@@ -2696,7 +2742,7 @@
         <v>20</v>
       </c>
       <c r="H97" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.2">
@@ -2719,7 +2765,7 @@
         <v>20</v>
       </c>
       <c r="H98" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.2">
@@ -2742,7 +2788,7 @@
         <v>20</v>
       </c>
       <c r="H99" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.2">
@@ -2765,7 +2811,7 @@
         <v>20</v>
       </c>
       <c r="H100" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>